<commit_message>
Everything is working till now 9thAug2024
</commit_message>
<xml_diff>
--- a/public/assets/backend-assets/images/SampleExcel/variants.xlsx
+++ b/public/assets/backend-assets/images/SampleExcel/variants.xlsx
@@ -81,9 +81,6 @@
     </r>
   </si>
   <si>
-    <t>Maruti</t>
-  </si>
-  <si>
     <t>Sigma 1.2L MT</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>6,5,3</t>
+  </si>
+  <si>
+    <t>Maruti Suzuki</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -600,34 +600,34 @@
         <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="E2" s="7">
         <v>751500</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L2" s="4">
         <v>5</v>
@@ -636,10 +636,10 @@
         <v>56</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>

</xml_diff>